<commit_message>
examinations table now generates properly
</commit_message>
<xml_diff>
--- a/slp-backend/report_templates/kzwa_template.xlsx
+++ b/slp-backend/report_templates/kzwa_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikiv\Praca Inżynierska\repository\SampleLab\slp-backend\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27A50F5-FD4D-438C-A11D-C24ED9AEED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C469F16F-F19A-4F2E-8F4F-7DDBEE92D49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -931,7 +931,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>